<commit_message>
Alteração no layout da tabela
</commit_message>
<xml_diff>
--- a/Contador Automático.xlsx
+++ b/Contador Automático.xlsx
@@ -80,13 +80,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -100,16 +113,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C5" totalsRowShown="0">
-  <autoFilter ref="A1:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="Count">
+    <tableColumn id="1" name="Count" dataDxfId="1">
       <calculatedColumnFormula>IF(ISNUMBER(OFFSET(A2,-1,0)),OFFSET(A2,-1,0)+1,1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" name="Nome"/>
     <tableColumn id="3" name="Telefone"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -378,28 +390,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <f ca="1">IF(ISNUMBER(OFFSET(A2,-1,0)),OFFSET(A2,-1,0)+1,1)</f>
         <v>1</v>
       </c>
@@ -408,7 +421,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <f ca="1">IF(ISNUMBER(OFFSET(A3,-1,0)),OFFSET(A3,-1,0)+1,1)</f>
         <v>2</v>
       </c>
@@ -417,7 +430,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <f ca="1">IF(ISNUMBER(OFFSET(A4,-1,0)),OFFSET(A4,-1,0)+1,1)</f>
         <v>3</v>
       </c>
@@ -426,7 +439,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <f ca="1">IF(ISNUMBER(OFFSET(A5,-1,0)),OFFSET(A5,-1,0)+1,1)</f>
         <v>4</v>
       </c>

</xml_diff>